<commit_message>
Did some play. No good result.
</commit_message>
<xml_diff>
--- a/Excel-Challenge-582_Pivot-on-Min-and-Max.xlsx
+++ b/Excel-Challenge-582_Pivot-on-Min-and-Max.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E60EA8D-E0ED-4ABF-806A-9AAE675F4C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9431724-9363-4D53-B599-259011D74658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19260" yWindow="100" windowWidth="19260" windowHeight="15410" activeTab="3" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
+    <workbookView xWindow="-19110" yWindow="40" windowWidth="19260" windowHeight="15410" activeTab="4" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
     <sheet name="Alt1" sheetId="3" r:id="rId3"/>
     <sheet name="Alt2" sheetId="5" r:id="rId4"/>
+    <sheet name="Play" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_d">EDA!$A$2:$A$26</definedName>
@@ -70,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +104,30 @@
   </si>
   <si>
     <t>Yet another variation on what I did. The variation is how the IDs are identified.</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>45353111|0.279861111111111</t>
+  </si>
+  <si>
+    <t>45353444|0.189583333333333</t>
+  </si>
+  <si>
+    <t>45356111|0.00347222222222222</t>
+  </si>
+  <si>
+    <t>45356333|0.00208333333333333</t>
+  </si>
+  <si>
+    <t>45356555|0.0895833333333333</t>
   </si>
 </sst>
 </file>
@@ -718,6 +743,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1107,8 +1135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E44F82-4113-4A07-80CF-D469F1B8AC68}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2235,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57E9371A-4D3A-4C0C-B67C-0DDBC9EB1521}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" activeCellId="1" sqref="E11 N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2795,6 +2823,1193 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8D1C6D-5AD4-4F4A-BCDD-A699E7F325A9}">
+  <dimension ref="A1:V41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34:M35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="20" max="20" width="12" customWidth="1"/>
+    <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1"/>
+      <c r="E1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B2">
+        <v>222</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.6694444444444444</v>
+      </c>
+      <c r="E2" s="1">
+        <v>45353</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="G2">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B3">
+        <v>222</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.77986111111111112</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45353</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B4">
+        <v>222</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45355</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B5">
+        <v>111</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.93958333333333333</v>
+      </c>
+      <c r="E5" s="1">
+        <v>45355</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="G5">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B6">
+        <v>333</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45356</v>
+      </c>
+      <c r="F6" s="3">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="G6">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B7">
+        <v>444</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45356</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B8">
+        <v>444</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.9194444444444444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B9">
+        <v>444</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B10">
+        <v>111</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B11">
+        <v>555</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B12">
+        <v>555</v>
+      </c>
+      <c r="C12" s="3">
+        <v>8.9583333333333334E-2</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12:G19">_xlfn.GROUPBY(_d,_t,_xlfn.VSTACK(_xleta.MIN,_xleta.MAX))</f>
+        <v>45353</v>
+      </c>
+      <c r="F12" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="G12">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="I12" t="str" cm="1">
+        <f t="array" ref="I12:O26">_xlfn.PIVOTBY(_d&amp;_id,_id,_t,_xlfn.VSTACK(_xleta.MIN,_xleta.MAX),0,0,,0)</f>
+        <v/>
+      </c>
+      <c r="J12" t="str">
+        <v/>
+      </c>
+      <c r="K12">
+        <v>111</v>
+      </c>
+      <c r="L12">
+        <v>222</v>
+      </c>
+      <c r="M12">
+        <v>333</v>
+      </c>
+      <c r="N12">
+        <v>444</v>
+      </c>
+      <c r="O12">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B13">
+        <v>222</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="E13">
+        <v>45353</v>
+      </c>
+      <c r="F13" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="G13">
+        <v>0.95</v>
+      </c>
+      <c r="I13" t="str">
+        <v>45353111</v>
+      </c>
+      <c r="J13" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K13">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <v/>
+      </c>
+      <c r="Q13" t="str" cm="1">
+        <f t="array" ref="Q13:V19">_xlfn.CHOOSECOLS(_xlfn._xlws.FILTER($I$13:$O$26,(J13:J26="MIN")),1,3,4,5,6,7)</f>
+        <v>45353111</v>
+      </c>
+      <c r="R13">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="S13" t="str">
+        <v/>
+      </c>
+      <c r="T13" t="str">
+        <v/>
+      </c>
+      <c r="U13" t="str">
+        <v/>
+      </c>
+      <c r="V13" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B14">
+        <v>111</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="E14">
+        <v>45355</v>
+      </c>
+      <c r="F14" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="str">
+        <v>45353111</v>
+      </c>
+      <c r="J14" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K14">
+        <v>0.95</v>
+      </c>
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <v/>
+      </c>
+      <c r="Q14" t="str">
+        <v>45353444</v>
+      </c>
+      <c r="R14" t="str">
+        <v/>
+      </c>
+      <c r="S14" t="str">
+        <v/>
+      </c>
+      <c r="T14" t="str">
+        <v/>
+      </c>
+      <c r="U14">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="V14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B15">
+        <v>555</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.60972222222222228</v>
+      </c>
+      <c r="E15">
+        <v>45355</v>
+      </c>
+      <c r="F15" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="G15">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="I15" t="str">
+        <v>45353444</v>
+      </c>
+      <c r="J15" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K15" t="str">
+        <v/>
+      </c>
+      <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="O15" t="str">
+        <v/>
+      </c>
+      <c r="Q15" t="str">
+        <v>45355222</v>
+      </c>
+      <c r="R15" t="str">
+        <v/>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15" t="str">
+        <v/>
+      </c>
+      <c r="U15" t="str">
+        <v/>
+      </c>
+      <c r="V15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>45353</v>
+      </c>
+      <c r="B16">
+        <v>444</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="E16">
+        <v>45356</v>
+      </c>
+      <c r="F16" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="G16">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I16" t="str">
+        <v>45353444</v>
+      </c>
+      <c r="J16" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K16" t="str">
+        <v/>
+      </c>
+      <c r="L16" t="str">
+        <v/>
+      </c>
+      <c r="M16" t="str">
+        <v/>
+      </c>
+      <c r="N16">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="O16" t="str">
+        <v/>
+      </c>
+      <c r="Q16" t="str">
+        <v>45355444</v>
+      </c>
+      <c r="R16" t="str">
+        <v/>
+      </c>
+      <c r="S16" t="str">
+        <v/>
+      </c>
+      <c r="T16" t="str">
+        <v/>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B17">
+        <v>333</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="E17">
+        <v>45356</v>
+      </c>
+      <c r="F17" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="G17">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="I17" t="str">
+        <v>45355222</v>
+      </c>
+      <c r="J17" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K17" t="str">
+        <v/>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17" t="str">
+        <v/>
+      </c>
+      <c r="N17" t="str">
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <v/>
+      </c>
+      <c r="Q17" t="str">
+        <v>45356111</v>
+      </c>
+      <c r="R17">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="S17" t="str">
+        <v/>
+      </c>
+      <c r="T17" t="str">
+        <v/>
+      </c>
+      <c r="U17" t="str">
+        <v/>
+      </c>
+      <c r="V17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>45355</v>
+      </c>
+      <c r="B18">
+        <v>222</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <v>Total</v>
+      </c>
+      <c r="F18" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="str">
+        <v>45355222</v>
+      </c>
+      <c r="J18" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K18" t="str">
+        <v/>
+      </c>
+      <c r="L18">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="M18" t="str">
+        <v/>
+      </c>
+      <c r="N18" t="str">
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <v/>
+      </c>
+      <c r="Q18" t="str">
+        <v>45356333</v>
+      </c>
+      <c r="R18" t="str">
+        <v/>
+      </c>
+      <c r="S18" t="str">
+        <v/>
+      </c>
+      <c r="T18">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="U18" t="str">
+        <v/>
+      </c>
+      <c r="V18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B19">
+        <v>333</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.20972222222222223</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Total</v>
+      </c>
+      <c r="F19" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="G19">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="I19" t="str">
+        <v>45355444</v>
+      </c>
+      <c r="J19" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K19" t="str">
+        <v/>
+      </c>
+      <c r="L19" t="str">
+        <v/>
+      </c>
+      <c r="M19" t="str">
+        <v/>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19" t="str">
+        <v/>
+      </c>
+      <c r="Q19" t="str">
+        <v>45356555</v>
+      </c>
+      <c r="R19" t="str">
+        <v/>
+      </c>
+      <c r="S19" t="str">
+        <v/>
+      </c>
+      <c r="T19" t="str">
+        <v/>
+      </c>
+      <c r="U19" t="str">
+        <v/>
+      </c>
+      <c r="V19">
+        <v>8.9583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B20">
+        <v>333</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="I20" t="str">
+        <v>45355444</v>
+      </c>
+      <c r="J20" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K20" t="str">
+        <v/>
+      </c>
+      <c r="L20" t="str">
+        <v/>
+      </c>
+      <c r="M20" t="str">
+        <v/>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B21">
+        <v>111</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.46319444444444446</v>
+      </c>
+      <c r="I21" t="str">
+        <v>45356111</v>
+      </c>
+      <c r="J21" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K21">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="L21" t="str">
+        <v/>
+      </c>
+      <c r="M21" t="str">
+        <v/>
+      </c>
+      <c r="N21" t="str">
+        <v/>
+      </c>
+      <c r="O21" t="str">
+        <v/>
+      </c>
+      <c r="Q21" t="str" cm="1">
+        <f t="array" ref="Q21:Q33">_xlfn.LET(_xlpm.z,_xlfn.DROP(_xlfn.TOCOL(_xlfn.MAP(_xlfn.ANCHORARRAY(Q13),_xlfn.LAMBDA(_xlpm.x,_xlfn.SINGLE(+Q27:_xlpm.x)&amp;"|"&amp;_xlpm.x))),1),_xlfn._xlws.FILTER(_xlpm.z,LEN(_xlpm.z)&gt;9))</f>
+        <v>45353111|0.279861111111111</v>
+      </c>
+      <c r="T21" t="str">
+        <f>LEFT(Q21,5)</f>
+        <v>45353</v>
+      </c>
+      <c r="U21" t="str">
+        <f>RIGHT(Q21,3)</f>
+        <v>111</v>
+      </c>
+      <c r="V21" t="str">
+        <f>_xlfn.TEXTAFTER(Q21,"|")</f>
+        <v>0.279861111111111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B22">
+        <v>111</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.64861111111111114</v>
+      </c>
+      <c r="I22" t="str">
+        <v>45356111</v>
+      </c>
+      <c r="J22" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K22">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="L22" t="str">
+        <v/>
+      </c>
+      <c r="M22" t="str">
+        <v/>
+      </c>
+      <c r="N22" t="str">
+        <v/>
+      </c>
+      <c r="O22" t="str">
+        <v/>
+      </c>
+      <c r="P22">
+        <f>LEN(Q22)</f>
+        <v>17</v>
+      </c>
+      <c r="Q22" t="str">
+        <v>45353444|45353444</v>
+      </c>
+      <c r="T22" t="str">
+        <f t="shared" ref="T22:T33" si="0">LEFT(Q22,5)</f>
+        <v>45353</v>
+      </c>
+      <c r="U22" t="str">
+        <f>RIGHT(Q22,3)</f>
+        <v>444</v>
+      </c>
+      <c r="V22" t="str">
+        <f t="shared" ref="V22:V33" si="1">_xlfn.TEXTAFTER(Q22,"|")</f>
+        <v>45353444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B23">
+        <v>111</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.35347222222222224</v>
+      </c>
+      <c r="I23" t="str">
+        <v>45356333</v>
+      </c>
+      <c r="J23" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K23" t="str">
+        <v/>
+      </c>
+      <c r="L23" t="str">
+        <v/>
+      </c>
+      <c r="M23">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="N23" t="str">
+        <v/>
+      </c>
+      <c r="O23" t="str">
+        <v/>
+      </c>
+      <c r="Q23" t="str">
+        <v>45353444|0.189583333333333</v>
+      </c>
+      <c r="T23" t="str">
+        <f t="shared" si="0"/>
+        <v>45353</v>
+      </c>
+      <c r="U23" t="str">
+        <f t="shared" ref="U23:U33" si="2">RIGHT(Q23,3)</f>
+        <v>333</v>
+      </c>
+      <c r="V23" t="str">
+        <f t="shared" si="1"/>
+        <v>0.189583333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B24">
+        <v>111</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="I24" t="str">
+        <v>45356333</v>
+      </c>
+      <c r="J24" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K24" t="str">
+        <v/>
+      </c>
+      <c r="L24" t="str">
+        <v/>
+      </c>
+      <c r="M24">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="N24" t="str">
+        <v/>
+      </c>
+      <c r="O24" t="str">
+        <v/>
+      </c>
+      <c r="Q24" t="str">
+        <v>45355222|45355222</v>
+      </c>
+      <c r="T24" t="str">
+        <f t="shared" si="0"/>
+        <v>45355</v>
+      </c>
+      <c r="U24" t="str">
+        <f t="shared" si="2"/>
+        <v>222</v>
+      </c>
+      <c r="V24" t="str">
+        <f t="shared" si="1"/>
+        <v>45355222</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B25">
+        <v>111</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I25" t="str">
+        <v>45356555</v>
+      </c>
+      <c r="J25" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K25" t="str">
+        <v/>
+      </c>
+      <c r="L25" t="str">
+        <v/>
+      </c>
+      <c r="M25" t="str">
+        <v/>
+      </c>
+      <c r="N25" t="str">
+        <v/>
+      </c>
+      <c r="O25">
+        <v>8.9583333333333334E-2</v>
+      </c>
+      <c r="Q25" t="str">
+        <v>45355222|0</v>
+      </c>
+      <c r="T25" t="str">
+        <f t="shared" si="0"/>
+        <v>45355</v>
+      </c>
+      <c r="U25" t="str">
+        <f t="shared" si="2"/>
+        <v>2|0</v>
+      </c>
+      <c r="V25" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45356</v>
+      </c>
+      <c r="B26">
+        <v>111</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.76597222222222228</v>
+      </c>
+      <c r="I26" t="str">
+        <v>45356555</v>
+      </c>
+      <c r="J26" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K26" t="str">
+        <v/>
+      </c>
+      <c r="L26" t="str">
+        <v/>
+      </c>
+      <c r="M26" t="str">
+        <v/>
+      </c>
+      <c r="N26" t="str">
+        <v/>
+      </c>
+      <c r="O26">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="Q26" t="str">
+        <v>45355444|45355444</v>
+      </c>
+      <c r="T26" t="str">
+        <f t="shared" si="0"/>
+        <v>45355</v>
+      </c>
+      <c r="U26" t="str">
+        <f t="shared" si="2"/>
+        <v>444</v>
+      </c>
+      <c r="V26" t="str">
+        <f t="shared" si="1"/>
+        <v>45355444</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q27" t="str">
+        <v>45355444|0</v>
+      </c>
+      <c r="T27" t="str">
+        <f t="shared" si="0"/>
+        <v>45355</v>
+      </c>
+      <c r="U27" t="str">
+        <f t="shared" si="2"/>
+        <v>4|0</v>
+      </c>
+      <c r="V27" t="str">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q28" t="str">
+        <v>45356111|45356111</v>
+      </c>
+      <c r="T28" t="str">
+        <f t="shared" si="0"/>
+        <v>45356</v>
+      </c>
+      <c r="U28" t="str">
+        <f t="shared" si="2"/>
+        <v>111</v>
+      </c>
+      <c r="V28" t="str">
+        <f t="shared" si="1"/>
+        <v>45356111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q29" t="str">
+        <v>45356111|0.00347222222222222</v>
+      </c>
+      <c r="T29" t="str">
+        <f t="shared" si="0"/>
+        <v>45356</v>
+      </c>
+      <c r="U29" t="str">
+        <f t="shared" si="2"/>
+        <v>222</v>
+      </c>
+      <c r="V29" t="str">
+        <f t="shared" si="1"/>
+        <v>0.00347222222222222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q30" t="str">
+        <v>45356333|45356333</v>
+      </c>
+      <c r="T30" t="str">
+        <f t="shared" si="0"/>
+        <v>45356</v>
+      </c>
+      <c r="U30" t="str">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+      <c r="V30" t="str">
+        <f t="shared" si="1"/>
+        <v>45356333</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q31" t="str">
+        <v>45356333|0.00208333333333333</v>
+      </c>
+      <c r="T31" t="str">
+        <f t="shared" si="0"/>
+        <v>45356</v>
+      </c>
+      <c r="U31" t="str">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+      <c r="V31" t="str">
+        <f t="shared" si="1"/>
+        <v>0.00208333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="Q32" t="str">
+        <v>45356555|45356555</v>
+      </c>
+      <c r="T32" t="str">
+        <f t="shared" si="0"/>
+        <v>45356</v>
+      </c>
+      <c r="U32" t="str">
+        <f t="shared" si="2"/>
+        <v>555</v>
+      </c>
+      <c r="V32" t="str">
+        <f t="shared" si="1"/>
+        <v>45356555</v>
+      </c>
+    </row>
+    <row r="33" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q33" t="str">
+        <v>45356555|0.0895833333333333</v>
+      </c>
+      <c r="T33" t="str">
+        <f t="shared" si="0"/>
+        <v>45356</v>
+      </c>
+      <c r="U33" t="str">
+        <f t="shared" si="2"/>
+        <v>333</v>
+      </c>
+      <c r="V33" t="str">
+        <f t="shared" si="1"/>
+        <v>0.0895833333333333</v>
+      </c>
+    </row>
+    <row r="35" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q35" t="s">
+        <v>14</v>
+      </c>
+      <c r="T35" s="1">
+        <v>45353</v>
+      </c>
+      <c r="U35" t="s">
+        <v>11</v>
+      </c>
+      <c r="V35" s="3">
+        <v>0.27986111111111101</v>
+      </c>
+    </row>
+    <row r="36" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q36" t="s">
+        <v>15</v>
+      </c>
+      <c r="T36" s="1">
+        <v>45353</v>
+      </c>
+      <c r="U36" t="s">
+        <v>12</v>
+      </c>
+      <c r="V36" s="3">
+        <v>0.18958333333333299</v>
+      </c>
+    </row>
+    <row r="37" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q37" t="s">
+        <v>16</v>
+      </c>
+      <c r="T37" s="1">
+        <v>45356</v>
+      </c>
+      <c r="U37" t="s">
+        <v>13</v>
+      </c>
+      <c r="V37" s="3">
+        <v>3.4722222222222199E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q38" t="s">
+        <v>17</v>
+      </c>
+      <c r="T38" s="1">
+        <v>45356</v>
+      </c>
+      <c r="U38" t="s">
+        <v>12</v>
+      </c>
+      <c r="V38" s="3">
+        <v>2.0833333333333298E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="Q39" t="s">
+        <v>18</v>
+      </c>
+      <c r="T39" s="1">
+        <v>45356</v>
+      </c>
+      <c r="U39" t="s">
+        <v>12</v>
+      </c>
+      <c r="V39" s="3">
+        <v>8.9583333333333307E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="T40" s="1"/>
+      <c r="V40" s="2"/>
+    </row>
+    <row r="41" spans="17:22" x14ac:dyDescent="0.3">
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Got a correct result, but not a good way to go.
</commit_message>
<xml_diff>
--- a/Excel-Challenge-582_Pivot-on-Min-and-Max.xlsx
+++ b/Excel-Challenge-582_Pivot-on-Min-and-Max.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9431724-9363-4D53-B599-259011D74658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24E021C-0D50-49BF-BD88-D4B6233EC2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19110" yWindow="40" windowWidth="19260" windowHeight="15410" activeTab="4" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>45356555|0.0895833333333333</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -194,7 +200,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -215,6 +221,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
@@ -2828,10 +2835,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8D1C6D-5AD4-4F4A-BCDD-A699E7F325A9}">
-  <dimension ref="A1:V41"/>
+  <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34:M35"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2841,6 +2848,7 @@
     <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5546875" customWidth="1"/>
     <col min="5" max="5" width="12.21875" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" customWidth="1"/>
     <col min="22" max="22" width="10" bestFit="1" customWidth="1"/>
   </cols>
@@ -3911,7 +3919,7 @@
         <v>45356555</v>
       </c>
     </row>
-    <row r="33" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:22" x14ac:dyDescent="0.3">
       <c r="Q33" t="str">
         <v>45356555|0.0895833333333333</v>
       </c>
@@ -3928,7 +3936,7 @@
         <v>0.0895833333333333</v>
       </c>
     </row>
-    <row r="35" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:22" x14ac:dyDescent="0.3">
       <c r="Q35" t="s">
         <v>14</v>
       </c>
@@ -3942,7 +3950,7 @@
         <v>0.27986111111111101</v>
       </c>
     </row>
-    <row r="36" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:22" x14ac:dyDescent="0.3">
       <c r="Q36" t="s">
         <v>15</v>
       </c>
@@ -3956,7 +3964,11 @@
         <v>0.18958333333333299</v>
       </c>
     </row>
-    <row r="37" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="K37" cm="1">
+        <f t="array" ref="K37:K39">_xlfn.UNIQUE(H44:H57)</f>
+        <v>45353</v>
+      </c>
       <c r="Q37" t="s">
         <v>16</v>
       </c>
@@ -3970,7 +3982,10 @@
         <v>3.4722222222222199E-3</v>
       </c>
     </row>
-    <row r="38" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>45355</v>
+      </c>
       <c r="Q38" t="s">
         <v>17</v>
       </c>
@@ -3984,7 +3999,10 @@
         <v>2.0833333333333298E-3</v>
       </c>
     </row>
-    <row r="39" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="K39">
+        <v>45356</v>
+      </c>
       <c r="Q39" t="s">
         <v>18</v>
       </c>
@@ -3998,12 +4016,315 @@
         <v>8.9583333333333307E-2</v>
       </c>
     </row>
-    <row r="40" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:22" x14ac:dyDescent="0.3">
       <c r="T40" s="1"/>
       <c r="V40" s="2"/>
     </row>
-    <row r="41" spans="17:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="8:22" x14ac:dyDescent="0.3">
       <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="H44" cm="1">
+        <f t="array" ref="H44:K59">_xlfn.PIVOTBY(_xlfn.HSTACK(_d,_id),,_t,_xlfn.VSTACK(_xleta.MAX,_xleta.MIN),)</f>
+        <v>45353</v>
+      </c>
+      <c r="I44">
+        <v>111</v>
+      </c>
+      <c r="J44" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M44">
+        <v>45353</v>
+      </c>
+      <c r="N44" t="s">
+        <v>19</v>
+      </c>
+      <c r="O44">
+        <v>444</v>
+      </c>
+      <c r="P44" s="3">
+        <f>_xlfn.MINIFS($K$44:$K$57,$H$44:$H$57,"="&amp;M44)</f>
+        <v>0.18958333333333333</v>
+      </c>
+    </row>
+    <row r="45" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="H45">
+        <v>45353</v>
+      </c>
+      <c r="I45">
+        <v>111</v>
+      </c>
+      <c r="J45" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="M45">
+        <v>45353</v>
+      </c>
+      <c r="N45" t="s">
+        <v>20</v>
+      </c>
+      <c r="O45">
+        <v>111</v>
+      </c>
+      <c r="P45" s="3">
+        <f>_xlfn.MAXIFS(K44:K57,H44:H57,"="&amp;M45)</f>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="46" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="H46">
+        <v>45353</v>
+      </c>
+      <c r="I46">
+        <v>444</v>
+      </c>
+      <c r="J46" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="M46">
+        <v>45355</v>
+      </c>
+      <c r="N46" t="s">
+        <v>19</v>
+      </c>
+      <c r="O46" s="12">
+        <v>222444</v>
+      </c>
+      <c r="P46" s="3">
+        <f t="shared" ref="P46" si="3">_xlfn.MINIFS($K$44:$K$57,$H$44:$H$57,"="&amp;M46)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="H47">
+        <v>45353</v>
+      </c>
+      <c r="I47">
+        <v>444</v>
+      </c>
+      <c r="J47" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="M47">
+        <v>45355</v>
+      </c>
+      <c r="N47" t="s">
+        <v>20</v>
+      </c>
+      <c r="O47">
+        <v>222</v>
+      </c>
+      <c r="P47" s="3">
+        <f t="shared" ref="P47" si="4">_xlfn.MAXIFS(K46:K59,H46:H59,"="&amp;M47)</f>
+        <v>0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="48" spans="8:22" x14ac:dyDescent="0.3">
+      <c r="H48">
+        <v>45355</v>
+      </c>
+      <c r="I48">
+        <v>222</v>
+      </c>
+      <c r="J48" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K48" s="3">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="M48">
+        <v>45356</v>
+      </c>
+      <c r="N48" t="s">
+        <v>19</v>
+      </c>
+      <c r="O48">
+        <v>333</v>
+      </c>
+      <c r="P48" s="3">
+        <f t="shared" ref="P48:P49" si="5">_xlfn.MINIFS($K$44:$K$57,$H$44:$H$57,"="&amp;M48)</f>
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H49">
+        <v>45355</v>
+      </c>
+      <c r="I49">
+        <v>222</v>
+      </c>
+      <c r="J49" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K49" s="2">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>45356</v>
+      </c>
+      <c r="N49" t="s">
+        <v>20</v>
+      </c>
+      <c r="O49" s="12">
+        <v>111555</v>
+      </c>
+      <c r="P49" s="3">
+        <f t="shared" ref="P49" si="6">_xlfn.MAXIFS(K48:K61,H48:H61,"="&amp;M49)</f>
+        <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="50" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H50">
+        <v>45355</v>
+      </c>
+      <c r="I50">
+        <v>444</v>
+      </c>
+      <c r="J50" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H51">
+        <v>45355</v>
+      </c>
+      <c r="I51">
+        <v>444</v>
+      </c>
+      <c r="J51" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H52">
+        <v>45356</v>
+      </c>
+      <c r="I52">
+        <v>111</v>
+      </c>
+      <c r="J52" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="53" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H53">
+        <v>45356</v>
+      </c>
+      <c r="I53">
+        <v>111</v>
+      </c>
+      <c r="J53" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K53" s="3">
+        <v>3.472222222222222E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H54">
+        <v>45356</v>
+      </c>
+      <c r="I54">
+        <v>333</v>
+      </c>
+      <c r="J54" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K54" s="3">
+        <v>0.63958333333333328</v>
+      </c>
+    </row>
+    <row r="55" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H55">
+        <v>45356</v>
+      </c>
+      <c r="I55">
+        <v>333</v>
+      </c>
+      <c r="J55" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K55" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H56">
+        <v>45356</v>
+      </c>
+      <c r="I56">
+        <v>555</v>
+      </c>
+      <c r="J56" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K56" s="3">
+        <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="57" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H57">
+        <v>45356</v>
+      </c>
+      <c r="I57">
+        <v>555</v>
+      </c>
+      <c r="J57" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K57" s="3">
+        <v>8.9583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H58" t="str">
+        <v>Total</v>
+      </c>
+      <c r="I58" t="str">
+        <v/>
+      </c>
+      <c r="J58" t="str">
+        <v>MAX</v>
+      </c>
+      <c r="K58">
+        <v>0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="59" spans="8:16" x14ac:dyDescent="0.3">
+      <c r="H59" t="str">
+        <v>Total</v>
+      </c>
+      <c r="I59" t="str">
+        <v/>
+      </c>
+      <c r="J59" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="K59">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I think I am done here.
</commit_message>
<xml_diff>
--- a/Excel-Challenge-582_Pivot-on-Min-and-Max.xlsx
+++ b/Excel-Challenge-582_Pivot-on-Min-and-Max.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24E021C-0D50-49BF-BD88-D4B6233EC2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D5CC76F-A23A-4BBB-8282-BE122880F18F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19110" yWindow="40" windowWidth="19260" windowHeight="15410" activeTab="4" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{BB796D0A-1929-4DDD-A038-93396BD327EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -1140,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E44F82-4113-4A07-80CF-D469F1B8AC68}">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1572,6 +1572,10 @@
       <c r="C23" s="2">
         <v>0.35347222222222224</v>
       </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
@@ -1583,31 +1587,6 @@
       <c r="C24" s="2">
         <v>0.96597222222222223</v>
       </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" t="str" cm="1">
-        <f t="array" ref="F24:L30">_xlfn.PIVOTBY(_d,_id,_t,_xlfn.VSTACK(_xleta.MIN,_xleta.MAX),0,0,,0)</f>
-        <v/>
-      </c>
-      <c r="G24" t="str">
-        <v/>
-      </c>
-      <c r="H24">
-        <v>111</v>
-      </c>
-      <c r="I24">
-        <v>222</v>
-      </c>
-      <c r="J24">
-        <v>333</v>
-      </c>
-      <c r="K24">
-        <v>444</v>
-      </c>
-      <c r="L24">
-        <v>555</v>
-      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -1619,26 +1598,30 @@
       <c r="C25" s="2">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="F25">
-        <v>45353</v>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" t="str" cm="1">
+        <f t="array" ref="F25:L31">_xlfn.PIVOTBY(_d,_id,_t,_xlfn.VSTACK(_xleta.MIN,_xleta.MAX),0,0,,0)</f>
+        <v/>
       </c>
       <c r="G25" t="str">
-        <v>MIN</v>
+        <v/>
       </c>
       <c r="H25">
-        <v>0.27986111111111112</v>
-      </c>
-      <c r="I25" t="str">
-        <v/>
-      </c>
-      <c r="J25" t="str">
-        <v/>
+        <v>111</v>
+      </c>
+      <c r="I25">
+        <v>222</v>
+      </c>
+      <c r="J25">
+        <v>333</v>
       </c>
       <c r="K25">
-        <v>0.18958333333333333</v>
-      </c>
-      <c r="L25" t="str">
-        <v/>
+        <v>444</v>
+      </c>
+      <c r="L25">
+        <v>555</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -1655,10 +1638,10 @@
         <v>45353</v>
       </c>
       <c r="G26" t="str">
-        <v>MAX</v>
+        <v>MIN</v>
       </c>
       <c r="H26">
-        <v>0.95</v>
+        <v>0.27986111111111112</v>
       </c>
       <c r="I26" t="str">
         <v/>
@@ -1667,7 +1650,7 @@
         <v/>
       </c>
       <c r="K26">
-        <v>0.9194444444444444</v>
+        <v>0.18958333333333333</v>
       </c>
       <c r="L26" t="str">
         <v/>
@@ -1675,22 +1658,22 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F27">
-        <v>45355</v>
+        <v>45353</v>
       </c>
       <c r="G27" t="str">
-        <v>MIN</v>
-      </c>
-      <c r="H27" t="str">
-        <v/>
-      </c>
-      <c r="I27">
-        <v>0</v>
+        <v>MAX</v>
+      </c>
+      <c r="H27">
+        <v>0.95</v>
+      </c>
+      <c r="I27" t="str">
+        <v/>
       </c>
       <c r="J27" t="str">
         <v/>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>0.9194444444444444</v>
       </c>
       <c r="L27" t="str">
         <v/>
@@ -1701,13 +1684,13 @@
         <v>45355</v>
       </c>
       <c r="G28" t="str">
-        <v>MAX</v>
+        <v>MIN</v>
       </c>
       <c r="H28" t="str">
         <v/>
       </c>
       <c r="I28">
-        <v>0.97777777777777775</v>
+        <v>0</v>
       </c>
       <c r="J28" t="str">
         <v/>
@@ -1721,25 +1704,25 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="F29">
-        <v>45356</v>
+        <v>45355</v>
       </c>
       <c r="G29" t="str">
-        <v>MIN</v>
-      </c>
-      <c r="H29">
-        <v>3.472222222222222E-3</v>
-      </c>
-      <c r="I29" t="str">
-        <v/>
-      </c>
-      <c r="J29">
-        <v>2.0833333333333333E-3</v>
-      </c>
-      <c r="K29" t="str">
-        <v/>
-      </c>
-      <c r="L29">
-        <v>8.9583333333333334E-2</v>
+        <v>MAX</v>
+      </c>
+      <c r="H29" t="str">
+        <v/>
+      </c>
+      <c r="I29">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="J29" t="str">
+        <v/>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="str">
+        <v/>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1747,22 +1730,521 @@
         <v>45356</v>
       </c>
       <c r="G30" t="str">
+        <v>MIN</v>
+      </c>
+      <c r="H30">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I30" t="str">
+        <v/>
+      </c>
+      <c r="J30">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="K30" t="str">
+        <v/>
+      </c>
+      <c r="L30">
+        <v>8.9583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>45356</v>
+      </c>
+      <c r="G31" t="str">
         <v>MAX</v>
       </c>
-      <c r="H30">
+      <c r="H31">
         <v>0.96597222222222223</v>
       </c>
-      <c r="I30" t="str">
-        <v/>
-      </c>
-      <c r="J30">
+      <c r="I31" t="str">
+        <v/>
+      </c>
+      <c r="J31">
         <v>0.63958333333333328</v>
       </c>
-      <c r="K30" t="str">
-        <v/>
-      </c>
-      <c r="L30">
+      <c r="K31" t="str">
+        <v/>
+      </c>
+      <c r="L31">
         <v>0.96597222222222223</v>
+      </c>
+    </row>
+    <row r="34" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="F34" t="str" cm="1">
+        <f t="array" ref="F34:I39">_xlfn.PIVOTBY(_id,_d,_t,_xleta.MAX,0,0,,0)</f>
+        <v/>
+      </c>
+      <c r="G34">
+        <v>45353</v>
+      </c>
+      <c r="H34">
+        <v>45355</v>
+      </c>
+      <c r="I34">
+        <v>45356</v>
+      </c>
+      <c r="K34" t="str" cm="1">
+        <f t="array" ref="K34:N39">_xlfn.PIVOTBY(_id,_d,_t,_xleta.MIN,0,0,,0)</f>
+        <v/>
+      </c>
+      <c r="L34">
+        <v>45353</v>
+      </c>
+      <c r="M34">
+        <v>45355</v>
+      </c>
+      <c r="N34">
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="35" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>111</v>
+      </c>
+      <c r="G35">
+        <v>0.95</v>
+      </c>
+      <c r="H35" t="str">
+        <v/>
+      </c>
+      <c r="I35">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="K35">
+        <v>111</v>
+      </c>
+      <c r="L35">
+        <v>0.27986111111111112</v>
+      </c>
+      <c r="M35" t="str">
+        <v/>
+      </c>
+      <c r="N35">
+        <v>3.472222222222222E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>222</v>
+      </c>
+      <c r="G36" t="str">
+        <v/>
+      </c>
+      <c r="H36">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="I36" t="str">
+        <v/>
+      </c>
+      <c r="K36">
+        <v>222</v>
+      </c>
+      <c r="L36" t="str">
+        <v/>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="F37">
+        <v>333</v>
+      </c>
+      <c r="G37" t="str">
+        <v/>
+      </c>
+      <c r="H37" t="str">
+        <v/>
+      </c>
+      <c r="I37">
+        <v>0.63958333333333328</v>
+      </c>
+      <c r="K37">
+        <v>333</v>
+      </c>
+      <c r="L37" t="str">
+        <v/>
+      </c>
+      <c r="M37" t="str">
+        <v/>
+      </c>
+      <c r="N37">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38">
+        <v>444</v>
+      </c>
+      <c r="G38">
+        <v>0.9194444444444444</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="str">
+        <v/>
+      </c>
+      <c r="K38">
+        <v>444</v>
+      </c>
+      <c r="L38">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>555</v>
+      </c>
+      <c r="G39" t="str">
+        <v/>
+      </c>
+      <c r="H39" t="str">
+        <v/>
+      </c>
+      <c r="I39">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="K39">
+        <v>555</v>
+      </c>
+      <c r="L39" t="str">
+        <v/>
+      </c>
+      <c r="M39" t="str">
+        <v/>
+      </c>
+      <c r="N39">
+        <v>8.9583333333333334E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G40" s="3">
+        <f>MAX(G35:G39)</f>
+        <v>0.95</v>
+      </c>
+      <c r="H40" s="3">
+        <f t="shared" ref="H40:I40" si="0">MAX(H35:H39)</f>
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="0"/>
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="J40" s="2"/>
+      <c r="L40" s="3">
+        <f>MIN(L35:L39)</f>
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="M40" s="3">
+        <f t="shared" ref="M40:N40" si="1">MIN(M35:M39)</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G41" t="str" cm="1">
+        <f t="array" ref="G41">_xlfn.ARRAYTOTEXT(INDEX($F$35:$F$39,_xlfn._xlws.FILTER($E$35:$E$39,G35:G39=G$40)))</f>
+        <v>111</v>
+      </c>
+      <c r="H41" t="str" cm="1">
+        <f t="array" ref="H41">_xlfn.ARRAYTOTEXT(INDEX($F$35:$F$39,_xlfn._xlws.FILTER($E$35:$E$39,H35:H39=H$40)))</f>
+        <v>222</v>
+      </c>
+      <c r="I41" t="str" cm="1">
+        <f t="array" ref="I41">_xlfn.ARRAYTOTEXT(INDEX($F$35:$F$39,_xlfn._xlws.FILTER($E$35:$E$39,I35:I39=I$40)))</f>
+        <v>111, 555</v>
+      </c>
+      <c r="L41" t="str" cm="1">
+        <f t="array" ref="L41">_xlfn.ARRAYTOTEXT(INDEX($F$35:$F$39,_xlfn._xlws.FILTER($E$35:$E$39,L35:L39=L$40)))</f>
+        <v>444</v>
+      </c>
+      <c r="M41" t="str" cm="1">
+        <f t="array" ref="M41">_xlfn.ARRAYTOTEXT(INDEX($F$35:$F$39,_xlfn._xlws.FILTER($E$35:$E$39,M35:M39=M$40)))</f>
+        <v>222, 444</v>
+      </c>
+      <c r="N41" t="str" cm="1">
+        <f t="array" ref="N41">_xlfn.ARRAYTOTEXT(INDEX($F$35:$F$39,_xlfn._xlws.FILTER($E$35:$E$39,N35:N39=N$40)))</f>
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G42" cm="1">
+        <f t="array" ref="G42:G44">_xlfn.VSTACK(G34,G40,G41)</f>
+        <v>45353</v>
+      </c>
+      <c r="H42" cm="1">
+        <f t="array" ref="H42:H44">_xlfn.VSTACK(H34,H40,H41)</f>
+        <v>45355</v>
+      </c>
+      <c r="I42" cm="1">
+        <f t="array" ref="I42:I44">_xlfn.VSTACK(I34,I40,I41)</f>
+        <v>45356</v>
+      </c>
+      <c r="L42" cm="1">
+        <f t="array" ref="L42:L44">_xlfn.VSTACK(L34,L40,L41)</f>
+        <v>45353</v>
+      </c>
+      <c r="M42" cm="1">
+        <f t="array" ref="M42:M44">_xlfn.VSTACK(M34,M40,M41)</f>
+        <v>45355</v>
+      </c>
+      <c r="N42" cm="1">
+        <f t="array" ref="N42:N44">_xlfn.VSTACK(N34,N40,N41)</f>
+        <v>45356</v>
+      </c>
+    </row>
+    <row r="43" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <v>0.95</v>
+      </c>
+      <c r="H43">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="I43">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="L43">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>2.0833333333333333E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="G44" t="str">
+        <v>111</v>
+      </c>
+      <c r="H44" t="str">
+        <v>222</v>
+      </c>
+      <c r="I44" t="str">
+        <v>111, 555</v>
+      </c>
+      <c r="L44" t="str">
+        <v>444</v>
+      </c>
+      <c r="M44" t="str">
+        <v>222, 444</v>
+      </c>
+      <c r="N44" t="str">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="46" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="F46" cm="1">
+        <f t="array" ref="F46:H48">TRANSPOSE(G42:I44)</f>
+        <v>45353</v>
+      </c>
+      <c r="G46">
+        <v>0.95</v>
+      </c>
+      <c r="H46" t="str">
+        <v>111</v>
+      </c>
+      <c r="L46" cm="1">
+        <f t="array" ref="L46:N48">TRANSPOSE(L42:N44)</f>
+        <v>45353</v>
+      </c>
+      <c r="M46">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="N46" t="str">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="47" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>45355</v>
+      </c>
+      <c r="G47">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="H47" t="str">
+        <v>222</v>
+      </c>
+      <c r="L47">
+        <v>45355</v>
+      </c>
+      <c r="M47">
+        <v>0</v>
+      </c>
+      <c r="N47" t="str">
+        <v>222, 444</v>
+      </c>
+    </row>
+    <row r="48" spans="5:14" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>45356</v>
+      </c>
+      <c r="G48">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="H48" t="str">
+        <v>111, 555</v>
+      </c>
+      <c r="L48">
+        <v>45356</v>
+      </c>
+      <c r="M48">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="N48" t="str">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="50" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F50" cm="1">
+        <f t="array" ref="F50:H55">_xlfn.VSTACK(_xlfn.ANCHORARRAY(L46),_xlfn.ANCHORARRAY(F46))</f>
+        <v>45353</v>
+      </c>
+      <c r="G50">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="H50" t="str">
+        <v>444</v>
+      </c>
+      <c r="J50" cm="1">
+        <f t="array" ref="J50:L55">_xlfn._xlws.SORT(_xlfn.ANCHORARRAY(F50),1)</f>
+        <v>45353</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0.18958333333333333</v>
+      </c>
+      <c r="L50" t="str">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="51" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>45355</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" t="str">
+        <v>222, 444</v>
+      </c>
+      <c r="J51">
+        <v>45353</v>
+      </c>
+      <c r="K51" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L51" t="str">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>45356</v>
+      </c>
+      <c r="G52">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="H52" t="str">
+        <v>333</v>
+      </c>
+      <c r="J52">
+        <v>45355</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0</v>
+      </c>
+      <c r="L52" t="str">
+        <v>222, 444</v>
+      </c>
+    </row>
+    <row r="53" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>45353</v>
+      </c>
+      <c r="G53">
+        <v>0.95</v>
+      </c>
+      <c r="H53" t="str">
+        <v>111</v>
+      </c>
+      <c r="J53">
+        <v>45355</v>
+      </c>
+      <c r="K53" s="3">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="L53" t="str">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="54" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>45355</v>
+      </c>
+      <c r="G54">
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="H54" t="str">
+        <v>222</v>
+      </c>
+      <c r="J54">
+        <v>45356</v>
+      </c>
+      <c r="K54" s="3">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="L54" t="str">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="6:12" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>45356</v>
+      </c>
+      <c r="G55">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="H55" t="str">
+        <v>111, 555</v>
+      </c>
+      <c r="J55">
+        <v>45356</v>
+      </c>
+      <c r="K55" s="2">
+        <v>0.96597222222222223</v>
+      </c>
+      <c r="L55" t="str">
+        <v>111, 555</v>
       </c>
     </row>
   </sheetData>
@@ -2837,8 +3319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8D1C6D-5AD4-4F4A-BCDD-A699E7F325A9}">
   <dimension ref="A1:V59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4157,7 +4639,7 @@
         <v>333</v>
       </c>
       <c r="P48" s="3">
-        <f t="shared" ref="P48:P49" si="5">_xlfn.MINIFS($K$44:$K$57,$H$44:$H$57,"="&amp;M48)</f>
+        <f t="shared" ref="P48" si="5">_xlfn.MINIFS($K$44:$K$57,$H$44:$H$57,"="&amp;M48)</f>
         <v>2.0833333333333333E-3</v>
       </c>
     </row>

</xml_diff>